<commit_message>
Thêm trạng thái để backup TaiKhoanGui, NhanVienGUI, KhachHangGUI
</commit_message>
<xml_diff>
--- a/excel/dsnv.xlsx
+++ b/excel/dsnv.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>staff_id</t>
   </si>
@@ -26,6 +26,18 @@
     <t>phone_number</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Huy Nguyen Anh</t>
+  </si>
+  <si>
+    <t>huyna@sgu.edu.vn</t>
+  </si>
+  <si>
+    <t>0909123123</t>
+  </si>
+  <si>
     <t>Minh Lu Quang</t>
   </si>
   <si>
@@ -48,12 +60,6 @@
   </si>
   <si>
     <t>ngoctn@sgu.edu.vn</t>
-  </si>
-  <si>
-    <t>tritranminh@sgu.edu.vn</t>
-  </si>
-  <si>
-    <t>ngocthetrang@sgu.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,75 +123,76 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>9</v>
+      <c r="E5" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>